<commit_message>
11ty Phase 2 + 3
</commit_message>
<xml_diff>
--- a/diaries/CEX_Diary_11ty.xlsx
+++ b/diaries/CEX_Diary_11ty.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lenap/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lenap/Documents/Git/cex-static-html/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36C4A9F-9200-4748-8F49-F63F2178862A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC1FD3F-37F7-D044-A3CD-9A2EAAED763A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,7 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>Session ID</t>
   </si>
@@ -73,9 +72,6 @@
   </si>
   <si>
     <t xml:space="preserve">Documentation Used </t>
-  </si>
-  <si>
-    <t>(e.g. ChatGPT, GitHub)</t>
   </si>
   <si>
     <t>Did you meet your goal this session? (Y/N)</t>
@@ -128,13 +124,81 @@
 Initialize project with basic routing and config: 2
 Apply a base theme: -
 Create the folder structure to hold data and pages: 2</t>
+  </si>
+  <si>
+    <t>11ty-2</t>
+  </si>
+  <si>
+    <t>Load ontology data into the SSG: 2
+Create templates to list teams and their members: 2
+Render one team detail page dynamically using ontology: 2
+Display one training schedule: 2</t>
+  </si>
+  <si>
+    <t>VS Code, Claude for file generation</t>
+  </si>
+  <si>
+    <t>Repeated template syntax errors
+Unclear error messages about exact syntax issues
+Filters liquid / nunjucks being very confusing</t>
+  </si>
+  <si>
+    <t>Partially - comfortable with data integration, but would need to reference Nunjucks syntax more carefully</t>
+  </si>
+  <si>
+    <t>Nunjucks templating syntax errors (date filter not available, compound conditionals)
+Template rendering failures requiring multiple iterations; Template file naming confusion (.md vs .njk vs .11tydata.js)</t>
+  </si>
+  <si>
+    <t>45-60</t>
+  </si>
+  <si>
+    <t>Error messages from 11ty build process; Documentation + ChatGPT; GitHub issues for similar problems</t>
+  </si>
+  <si>
+    <t>Had to restart dev server and clean cache several times; syntax erros; relationships between pages, permalinks etc wasnt clear from documentation</t>
+  </si>
+  <si>
+    <t>11ty's pagination isn't intuitive</t>
+  </si>
+  <si>
+    <t>https://www.11ty.dev/docs/permalinks/; https://www.11ty.dev/docs/data/</t>
+  </si>
+  <si>
+    <t>11ty-3</t>
+  </si>
+  <si>
+    <t>Display upcoming tournaments in a calendar-style list: 2
+Connect team participation to tournament listings: 2
+Build a basic membership application form (HTML only, no backend): 3</t>
+  </si>
+  <si>
+    <t>VS Code, GitHub Copilot</t>
+  </si>
+  <si>
+    <t>Data lookup for teams/coaches, output conflicts, template scoping</t>
+  </si>
+  <si>
+    <t>Output path conflicts, Nunjucks filters being confusing</t>
+  </si>
+  <si>
+    <t>For Tournaments and Training Data lookup always returned first item; fixed by correct filter usage and scoping</t>
+  </si>
+  <si>
+    <t>Documentation + GitHub Copilot</t>
+  </si>
+  <si>
+    <t>Data not displaying as expected, output conflicts</t>
+  </si>
+  <si>
+    <t>https://www.11ty.dev/docs/filters/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +237,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -206,10 +278,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -226,26 +299,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -551,7 +641,7 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -595,16 +685,16 @@
         <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -622,24 +712,24 @@
         <v>8</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="8" customFormat="1" ht="255" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="9">
         <v>45827</v>
@@ -651,16 +741,16 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I2" s="8">
         <v>30</v>
@@ -669,39 +759,152 @@
         <v>0</v>
       </c>
       <c r="K2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="8" t="s">
+      <c r="N2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="P2" s="8">
         <v>20</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R2" s="13"/>
       <c r="S2" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="176" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="14">
+        <v>45843</v>
+      </c>
+      <c r="C3" s="15">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="D3" s="16">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3">
+        <v>15</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T3" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="86" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="14">
+        <v>45849</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D4" s="16">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4">
+        <v>40</v>
+      </c>
+      <c r="J4">
+        <v>30</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="P4">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="S4" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="5" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -778,6 +981,10 @@
       <c r="E24" s="6"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H4" r:id="rId1" xr:uid="{13C25FAE-2724-464A-B20D-2625AAC87B69}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added missing diary and survey files
</commit_message>
<xml_diff>
--- a/diaries/CEX_Diary_11ty.xlsx
+++ b/diaries/CEX_Diary_11ty.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lenap/Documents/Git/cex-static-html/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC1FD3F-37F7-D044-A3CD-9A2EAAED763A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5391F550-A534-7445-A17C-102F2D179D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28580" yWindow="780" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="69">
   <si>
     <t>Session ID</t>
   </si>
@@ -192,6 +192,74 @@
   </si>
   <si>
     <t>https://www.11ty.dev/docs/filters/</t>
+  </si>
+  <si>
+    <t>11ty-4</t>
+  </si>
+  <si>
+    <t>News/blog list: 3
+Homepage call to join: 3
+Static pages (About/Contact): 3
+Navbar: 3</t>
+  </si>
+  <si>
+    <t>Getting collections to work with Markdown required trial and error; homepage layout needed overrides for callout section</t>
+  </si>
+  <si>
+    <t>https://www.11ty.dev/docs/collections/
+https://www.11ty.dev/docs/layouts/</t>
+  </si>
+  <si>
+    <t>Collection config &amp; layout overrides needed</t>
+  </si>
+  <si>
+    <t>Markdown rendering worked well, but layout scoping needed multiple attempts</t>
+  </si>
+  <si>
+    <t>11ty docs, GitHub Copilot, ChatGPT</t>
+  </si>
+  <si>
+    <t>Collection setup</t>
+  </si>
+  <si>
+    <t>partially</t>
+  </si>
+  <si>
+    <t>11ty-5</t>
+  </si>
+  <si>
+    <t>GitHub Actions setup: 3
+Public directory deployment: 3
+Fix broken pages: 3
+Validate hosted site: 3</t>
+  </si>
+  <si>
+    <t>VS Code, GitHub Desktop</t>
+  </si>
+  <si>
+    <t>None major — GitHub deployment was smooth after reading a guide</t>
+  </si>
+  <si>
+    <t>GitHub Pages + Actions docs
+https://www.11ty.dev/docs/deployment/; https://www.dawidsblog.com/posts/tutorial_11ty_github_pages/</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>mostly config lookup</t>
+  </si>
+  <si>
+    <t>GitHub Pages deployment tutorial</t>
+  </si>
+  <si>
+    <t>Slight confusion about public folder and .nojekyll, quickly resolved</t>
+  </si>
+  <si>
+    <t>Yes!</t>
   </si>
 </sst>
 </file>
@@ -282,7 +350,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -333,6 +401,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -640,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -905,13 +985,123 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
+    <row r="5" spans="1:20" s="22" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="23">
+        <v>45858</v>
+      </c>
+      <c r="C5" s="24">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D5" s="24">
+        <v>0.84375</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="22">
+        <v>45</v>
+      </c>
+      <c r="J5" s="22">
+        <v>20</v>
+      </c>
+      <c r="K5" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="N5" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="P5" s="22">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="S5" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="T5" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" s="22" customFormat="1" ht="144" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="23">
+        <v>45861</v>
+      </c>
+      <c r="C6" s="24">
+        <v>0.79861111111111116</v>
+      </c>
+      <c r="D6" s="24">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" s="22">
+        <v>15</v>
+      </c>
+      <c r="J6" s="22">
+        <v>5</v>
+      </c>
+      <c r="K6" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="L6" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="M6" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="O6" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="P6" s="22">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="S6" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="T6" s="22" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="7" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="E7" s="5"/>

</xml_diff>